<commit_message>
Update ui and aidat template
</commit_message>
<xml_diff>
--- a/biyos/aidat/template/aidat.xlsx
+++ b/biyos/aidat/template/aidat.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mustafa Kaptan\git\biyos-app\biyos\aidat\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="295"/>
   </bookViews>
   <sheets>
     <sheet name="2016 - Mart" sheetId="1" r:id="rId1"/>
@@ -78,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,18 +205,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,6 +219,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,38 +513,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="12.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="9.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -577,8 +572,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+    <row r="4" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
@@ -590,21 +585,21 @@
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+    <row r="5" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="5"/>
@@ -616,21 +611,21 @@
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+    <row r="7" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="5"/>
@@ -642,21 +637,21 @@
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+    <row r="9" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
         <v>7</v>
       </c>
       <c r="B10" s="5"/>
@@ -668,21 +663,21 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+    <row r="11" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
         <v>9</v>
       </c>
       <c r="B12" s="5"/>
@@ -694,21 +689,21 @@
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+    <row r="13" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
         <v>10</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
         <v>11</v>
       </c>
       <c r="B14" s="5"/>
@@ -720,21 +715,21 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+    <row r="15" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10">
         <v>12</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="5"/>
@@ -746,21 +741,21 @@
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+    <row r="17" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10">
         <v>14</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
         <v>15</v>
       </c>
       <c r="B18" s="5"/>
@@ -772,21 +767,21 @@
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
+    <row r="19" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10">
         <v>16</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
-    </row>
-    <row r="20" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
         <v>17</v>
       </c>
       <c r="B20" s="5"/>
@@ -798,21 +793,21 @@
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
+    <row r="21" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10">
         <v>18</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
-    </row>
-    <row r="22" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
         <v>19</v>
       </c>
       <c r="B22" s="5"/>
@@ -824,21 +819,21 @@
       <c r="H22" s="5"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
+    <row r="23" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10">
         <v>20</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
         <v>21</v>
       </c>
       <c r="B24" s="5"/>
@@ -850,21 +845,21 @@
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+    <row r="25" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10">
         <v>22</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="16"/>
-    </row>
-    <row r="26" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9">
         <v>23</v>
       </c>
       <c r="B26" s="5"/>
@@ -876,52 +871,52 @@
       <c r="H26" s="5"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+    <row r="27" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10">
         <v>24</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10" t="s">
+      <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9" ht="12.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:9" ht="56.1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="12" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" ht="9.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:9" ht="56.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -949,8 +944,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
+    <row r="32" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9">
         <v>1</v>
       </c>
       <c r="B32" s="5"/>
@@ -962,21 +957,21 @@
       <c r="H32" s="5"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+    <row r="33" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="10">
         <v>2</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="16"/>
-    </row>
-    <row r="34" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9">
         <v>3</v>
       </c>
       <c r="B34" s="5"/>
@@ -988,21 +983,21 @@
       <c r="H34" s="5"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+    <row r="35" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="10">
         <v>4</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="16"/>
-    </row>
-    <row r="36" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="9">
         <v>5</v>
       </c>
       <c r="B36" s="5"/>
@@ -1014,21 +1009,21 @@
       <c r="H36" s="5"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+    <row r="37" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="10">
         <v>6</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="16"/>
-    </row>
-    <row r="38" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="9">
         <v>7</v>
       </c>
       <c r="B38" s="5"/>
@@ -1040,21 +1035,21 @@
       <c r="H38" s="5"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+    <row r="39" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10">
         <v>8</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="16"/>
-    </row>
-    <row r="40" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="9">
         <v>9</v>
       </c>
       <c r="B40" s="5"/>
@@ -1066,21 +1061,21 @@
       <c r="H40" s="5"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
+    <row r="41" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10">
         <v>10</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="16"/>
-    </row>
-    <row r="42" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="9">
         <v>11</v>
       </c>
       <c r="B42" s="5"/>
@@ -1092,21 +1087,21 @@
       <c r="H42" s="5"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14">
+    <row r="43" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10">
         <v>12</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="16"/>
-    </row>
-    <row r="44" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="9">
         <v>13</v>
       </c>
       <c r="B44" s="5"/>
@@ -1118,21 +1113,21 @@
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14">
+    <row r="45" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10">
         <v>14</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="16"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="13">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="9">
         <v>15</v>
       </c>
       <c r="B46" s="5"/>
@@ -1144,21 +1139,21 @@
       <c r="H46" s="5"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
+    <row r="47" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="10">
         <v>16</v>
       </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="16"/>
-    </row>
-    <row r="48" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="13">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="12"/>
+    </row>
+    <row r="48" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="9">
         <v>17</v>
       </c>
       <c r="B48" s="5"/>
@@ -1170,21 +1165,21 @@
       <c r="H48" s="5"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14">
+    <row r="49" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10">
         <v>18</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="16"/>
-    </row>
-    <row r="50" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="12"/>
+    </row>
+    <row r="50" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="9">
         <v>19</v>
       </c>
       <c r="B50" s="5"/>
@@ -1196,21 +1191,21 @@
       <c r="H50" s="5"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14">
+    <row r="51" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="10">
         <v>20</v>
       </c>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="16"/>
-    </row>
-    <row r="52" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="9">
         <v>21</v>
       </c>
       <c r="B52" s="5"/>
@@ -1222,21 +1217,21 @@
       <c r="H52" s="5"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
+    <row r="53" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="10">
         <v>22</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="16"/>
-    </row>
-    <row r="54" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="12"/>
+    </row>
+    <row r="54" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="9">
         <v>23</v>
       </c>
       <c r="B54" s="5"/>
@@ -1248,31 +1243,31 @@
       <c r="H54" s="5"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="14">
+    <row r="55" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="10">
         <v>24</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="16"/>
-    </row>
-    <row r="56" spans="1:9" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="12"/>
+    </row>
+    <row r="56" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1285,7 +1280,8 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:I29"/>
   </mergeCells>
-  <pageMargins left="0.56944444444444398" right="0.41666666666666702" top="0.41666666666666702" bottom="0.41666666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup firstPageNumber="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>